<commit_message>
Cleaned up repo, added mosfet driver
removed old folders, renamed files to make more sense, made search path simpler and put all symbols/schematics in one place. Made a simple bjt totem pole mosfet driver and started adding to the BOM
</commit_message>
<xml_diff>
--- a/Data/Wind Turbine BOM1.xlsx
+++ b/Data/Wind Turbine BOM1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\BCIT\7000\WindChargeController-Capstone2024\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6120B8-4CCD-4798-8F48-1D61B6FEFC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CD8C3A-E1A2-4ABE-B140-FC693B9574A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -151,6 +151,27 @@
   <si>
     <t>https://www.digikey.ca/en/products/detail/cornell-dubilier-illinois-capacitor/108CKE063M/5343985</t>
   </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW12061M00FKEA/1176986</t>
+  </si>
+  <si>
+    <t>CRCW12061M00FKEA</t>
+  </si>
+  <si>
+    <t>2N5210 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/central-semiconductor-corp/2n5210-pbfree/4806912</t>
+  </si>
+  <si>
+    <t>bjt for mosfet driver</t>
+  </si>
+  <si>
+    <t>2N5087 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/central-semiconductor-corp/2n5087-pbfree/4806906</t>
+  </si>
 </sst>
 </file>
 
@@ -159,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -220,6 +241,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -307,10 +335,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -366,6 +395,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -387,17 +425,15 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,7 +654,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -652,7 +688,7 @@
       </c>
     </row>
     <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -660,19 +696,19 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -754,13 +790,13 @@
       <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="20">
         <v>5</v>
       </c>
       <c r="F11" s="13"/>
@@ -849,7 +885,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -996,15 +1032,25 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="B16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="9">
+        <v>5</v>
+      </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="13">
+        <v>0.16</v>
+      </c>
       <c r="H16" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="12"/>
@@ -1035,15 +1081,25 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="B17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5</v>
+      </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="13">
+        <v>0.79</v>
+      </c>
       <c r="H17" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.95</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="12"/>
@@ -1074,15 +1130,25 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="9">
+        <v>5</v>
+      </c>
       <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="13">
+        <v>0.69</v>
+      </c>
       <c r="H18" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="12"/>
@@ -1233,12 +1299,12 @@
       <c r="E22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="23">
         <f>SUM(H11:H21)</f>
-        <v>34.450000000000003</v>
+        <v>42.650000000000006</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
@@ -1271,12 +1337,12 @@
       <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="23">
         <f>F22*0.12</f>
-        <v>4.1340000000000003</v>
+        <v>5.1180000000000003</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
@@ -1309,12 +1375,12 @@
       <c r="E24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="26">
         <f>SUM(F22:H23)</f>
-        <v>38.584000000000003</v>
+        <v>47.768000000000008</v>
       </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="25"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -34016,6 +34082,9 @@
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="F24:H24"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{AA199301-BD1B-4E57-81D2-B284FF4635AF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started KiCad work, working on BOM
</commit_message>
<xml_diff>
--- a/Data/Wind Turbine BOM1.xlsx
+++ b/Data/Wind Turbine BOM1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\BCIT\7000\WindChargeController-Capstone2024\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CD8C3A-E1A2-4ABE-B140-FC693B9574A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A77BDC-17E1-4436-8E95-D438E111966B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="-16200" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,24 +134,6 @@
     <t>resistor for DCDC</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/en/products/detail/cornell-dubilier-illinois-capacitor/107CKE100MLQ/5410737</t>
-  </si>
-  <si>
-    <t>107CKE100MLQ</t>
-  </si>
-  <si>
-    <t>decoupling cap for input</t>
-  </si>
-  <si>
-    <t>decoupling cap for output</t>
-  </si>
-  <si>
-    <t>108CKE063M</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/cornell-dubilier-illinois-capacitor/108CKE063M/5343985</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/en/products/detail/vishay-dale/CRCW12061M00FKEA/1176986</t>
   </si>
   <si>
@@ -171,6 +153,24 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/central-semiconductor-corp/2n5087-pbfree/4806906</t>
+  </si>
+  <si>
+    <t>decoupling capacitor for in/output</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/panasonic-electronic-components/EEU-FS2A151/9597035</t>
+  </si>
+  <si>
+    <t>EEU-FS2A151</t>
+  </si>
+  <si>
+    <t>diode for DCDC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/SI7336ADP-T1-GE3/SI7336ADP-T1-GE3CT-ND/3758703?WT.z_cid=ref_netcomponents_dkc_buynow&amp;utm_source=netcomponents&amp;utm_medium=aggregator&amp;utm_campaign=buynow</t>
+  </si>
+  <si>
+    <t>SI7336ADP-T1-GE3</t>
   </si>
 </sst>
 </file>
@@ -339,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -404,6 +404,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -425,11 +431,8 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -654,7 +657,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -688,7 +691,7 @@
       </c>
     </row>
     <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="24" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -696,19 +699,19 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -794,7 +797,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E11" s="20">
         <v>5</v>
@@ -836,7 +839,7 @@
         <f t="shared" ref="A12:A21" si="0">A11+1</f>
         <v>2</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="11" t="s">
@@ -885,7 +888,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -931,28 +934,23 @@
     </row>
     <row r="14" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>33</v>
+      <c r="B14" s="22" t="s">
+        <v>44</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>34</v>
+      <c r="C14" s="19" t="s">
+        <v>45</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>35</v>
+      <c r="D14" s="31" t="s">
+        <v>28</v>
       </c>
-      <c r="E14" s="9">
-        <v>5</v>
-      </c>
+      <c r="E14" s="20"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="13">
-        <v>1.05</v>
-      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="13">
         <f t="shared" si="1"/>
-        <v>5.25</v>
+        <v>0</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="12"/>
@@ -980,28 +978,25 @@
     </row>
     <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>38</v>
+      <c r="B15" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
-      <c r="E15" s="9">
-        <v>5</v>
-      </c>
+      <c r="E15" s="9"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13">
-        <v>1.96</v>
+        <v>1.85</v>
       </c>
       <c r="H15" s="13">
         <f t="shared" si="1"/>
-        <v>9.8000000000000007</v>
+        <v>0</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="12"/>
@@ -1033,10 +1028,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>32</v>
@@ -1082,13 +1077,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E17" s="9">
         <v>5</v>
@@ -1131,13 +1126,13 @@
         <v>8</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>44</v>
+      <c r="C18" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E18" s="9">
         <v>5</v>
@@ -1299,12 +1294,12 @@
       <c r="E22" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="25">
         <f>SUM(H11:H21)</f>
-        <v>42.650000000000006</v>
+        <v>27.599999999999998</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="25"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
@@ -1337,12 +1332,12 @@
       <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="25">
         <f>F22*0.12</f>
-        <v>5.1180000000000003</v>
+        <v>3.3119999999999998</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="25"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
@@ -1375,12 +1370,12 @@
       <c r="E24" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="28">
         <f>SUM(F22:H23)</f>
-        <v>47.768000000000008</v>
+        <v>30.911999999999999</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -34084,6 +34079,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{AA199301-BD1B-4E57-81D2-B284FF4635AF}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{DEFC2C15-712D-4C3E-85AE-0BCE3579C27A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>